<commit_message>
Update my personal log
</commit_message>
<xml_diff>
--- a/LogJason.xlsx
+++ b/LogJason.xlsx
@@ -1,41 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deleb\Desktop\Avanced System Security\Kaggle-Microsoft-Malware-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B3494A-1353-4B55-A838-88EDDC588C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BBD77AD-676E-4538-91A3-615FC062B49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
   <si>
     <t>10.20.19</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Activities</t>
-  </si>
-  <si>
     <t>Experimentation with data summary and statistic, initial cleaning of useless feature, selection of useful features, personal study of strategies for the time serie problem</t>
   </si>
   <si>
@@ -67,13 +73,19 @@
   </si>
   <si>
     <t>Notebook refactoring, initial feature engineering and balancing for testing feature importance</t>
+  </si>
+  <si>
+    <t>11.14.19</t>
+  </si>
+  <si>
+    <t>Notebook refactoring, initial algorithm evaluatiojn section writing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -387,35 +399,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" customWidth="1"/>
-    <col min="2" max="2" width="71.90625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="29.1">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="57.95">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -423,7 +435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="29.1">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -431,7 +443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="29.1">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -439,7 +451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="29.1">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -447,12 +459,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="29.1">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Big update, code runned
</commit_message>
<xml_diff>
--- a/LogJason.xlsx
+++ b/LogJason.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deleb\Desktop\Avanced System Security\Kaggle-Microsoft-Malware-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64F2730-0FC8-457A-8F6D-B02FCAD6270E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6F2895-EA61-4929-A304-E684A64E09C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -84,9 +84,6 @@
     <t>11.20.19</t>
   </si>
   <si>
-    <t>Added new features as a feature engineering task, algorithm testing code cleanup, initial writing of documentation</t>
-  </si>
-  <si>
     <t>Collaborated with Yibo on feature balancing and engineering</t>
   </si>
   <si>
@@ -109,6 +106,15 @@
   </si>
   <si>
     <t>Finished feature engineering with Yibo, introduced more visualization methods, improved grid research and tested NN on real machine. Overall completion of the code part in the notebook</t>
+  </si>
+  <si>
+    <t>12.07.19</t>
+  </si>
+  <si>
+    <t>Finished notebook final code run, finished code part, refactored all notebook with new outline, started writing documentation</t>
+  </si>
+  <si>
+    <t>Added new features as a feature engineering task, algorithm testing code cleanup, initial writing of coumentation</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -510,39 +516,47 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished notebook documentation (needs revising)
</commit_message>
<xml_diff>
--- a/LogJason.xlsx
+++ b/LogJason.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deleb\Desktop\Avanced System Security\Kaggle-Microsoft-Malware-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9D60CF-C5F8-49B4-BFA4-BDD05022F3CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83317CE3-7D67-4C4C-9BFE-CCD1E0C04BA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Progresses in notebook documentation writing (finished up to algo. Spot-checking section)</t>
+  </si>
+  <si>
+    <t>12.10.19</t>
+  </si>
+  <si>
+    <t>Finished Notebook documentation (Needs revising)</t>
   </si>
 </sst>
 </file>
@@ -447,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,6 +593,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>